<commit_message>
update new mapping and reduce method
</commit_message>
<xml_diff>
--- a/tabula.xlsx
+++ b/tabula.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vutuanhai/Documents/GitHub/Quojo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B378CBE4-B2E4-D341-BFF2-1F2042F45F71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B345236-D225-5544-AE82-6B206C86A63D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="0" windowWidth="28040" windowHeight="16800" xr2:uid="{9D8BCA9F-CC44-044D-8942-29B598D43168}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="65">
   <si>
     <t>Gate</t>
   </si>
@@ -68,16 +69,7 @@
     <t>Z</t>
   </si>
   <si>
-    <t>-Y</t>
-  </si>
-  <si>
-    <t>-X</t>
-  </si>
-  <si>
-    <t>X'</t>
-  </si>
-  <si>
-    <t>Y'</t>
+    <t>I</t>
   </si>
   <si>
     <t>IX</t>
@@ -125,17 +117,128 @@
     <t>ZZ</t>
   </si>
   <si>
-    <t>-YY</t>
-  </si>
-  <si>
-    <t>-XZ</t>
+    <t>X,Y</t>
+  </si>
+  <si>
+    <t>II</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>[0.707,0.707]</t>
+  </si>
+  <si>
+    <t>[X,Y]</t>
+  </si>
+  <si>
+    <t>[Y,X]</t>
+  </si>
+  <si>
+    <t>[0.707,-0.707]</t>
+  </si>
+  <si>
+    <t>RX(\theta)</t>
+  </si>
+  <si>
+    <t>RY(\theta)</t>
+  </si>
+  <si>
+    <t>RZ(\theta)</t>
+  </si>
+  <si>
+    <t>Y,X</t>
+  </si>
+  <si>
+    <t>[Y,Z]</t>
+  </si>
+  <si>
+    <t>[Z,Y]</t>
+  </si>
+  <si>
+    <t>[X,Z]</t>
+  </si>
+  <si>
+    <t>[Z,X]</t>
+  </si>
+  <si>
+    <t>Lambda</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>-i</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>[cos(\theta/2), sin(\theta/2)]</t>
+  </si>
+  <si>
+    <t>[cos(\theta/2), -sin(\theta/2)]</t>
+  </si>
+  <si>
+    <t>XI/IX</t>
+  </si>
+  <si>
+    <t>YI/IY</t>
+  </si>
+  <si>
+    <t>ZI/IZ</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -143,16 +246,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -160,13 +282,159 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -501,248 +769,836 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{738C72C8-C828-2F4E-9CF8-48BAE1CA406F}">
-  <dimension ref="D4:F28"/>
+  <dimension ref="D4:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="138" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="4.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="4" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D4" s="1" t="s">
+    <row r="4" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D4" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1" t="s">
+      <c r="G4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="6" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
+      <c r="G5" s="2">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="2">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
+      <c r="F8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="2">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K10" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="2">
+        <v>1</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="2">
+        <v>1</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K12" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="1" t="s">
+      <c r="F13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="J13" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
+      <c r="F14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="J14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="2">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K15" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" x14ac:dyDescent="0.2">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K16" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E17" s="15" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
+      <c r="F17" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="G17" s="15">
+        <v>1</v>
+      </c>
+      <c r="H17" s="5"/>
+      <c r="I17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K17" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="O17" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="P17" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D18" s="2"/>
+      <c r="E18" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="G18" s="14">
+        <v>1</v>
+      </c>
+      <c r="H18" s="6"/>
+      <c r="I18" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="O18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="P18" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D19" s="2"/>
+      <c r="E19" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="14">
+        <v>1</v>
+      </c>
+      <c r="H19" s="6"/>
+      <c r="I19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="P19" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D20" s="2"/>
+      <c r="E20" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G20" s="14">
+        <v>1</v>
+      </c>
+      <c r="H20" s="6"/>
+      <c r="I20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="K20" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="O20" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="P20" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D21" s="2"/>
+      <c r="E21" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F21" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21" s="14">
+        <v>1</v>
+      </c>
+      <c r="H21" s="6"/>
+      <c r="I21" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="O21" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="P21" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D22" s="2"/>
+      <c r="E22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F22" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G22" s="15">
+        <v>1</v>
+      </c>
+      <c r="H22" s="6"/>
+      <c r="I22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="O22" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="P22" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G23" s="2">
+        <v>1</v>
+      </c>
+      <c r="H23" s="6"/>
+      <c r="I23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J23" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D11" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="K23" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="P23" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1</v>
+      </c>
+      <c r="H24" s="6"/>
+      <c r="I24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="O24" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="P24" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G25" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H25" s="6"/>
+      <c r="I25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J25" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
+      <c r="K25" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="O25" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="P25" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="26" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G26" s="2">
+        <v>1</v>
+      </c>
+      <c r="H26" s="6"/>
+      <c r="I26" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M26" s="2"/>
+      <c r="N26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="O26" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P26" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="2">
+        <v>-1</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="I27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="K27" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="M27" s="2"/>
+      <c r="N27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="P27" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="28" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G28" s="2">
+        <v>1</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="I28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="M28" s="2"/>
+      <c r="N28" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="P28" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D29" s="2"/>
+      <c r="E29" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="15">
+        <v>1</v>
+      </c>
+      <c r="H29" s="6"/>
+      <c r="I29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M29" s="2"/>
+      <c r="N29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P29" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="14" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D15" s="1"/>
-      <c r="E15" s="1" t="s">
+      <c r="G30" s="2">
+        <v>1</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="P30" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F31" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D16" s="1"/>
-      <c r="E16" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="G31" s="2">
+        <v>1</v>
+      </c>
+      <c r="H31" s="6"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="10"/>
+      <c r="M31" s="2"/>
+      <c r="N31" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="P31" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="4:16" x14ac:dyDescent="0.2">
+      <c r="D32" s="2"/>
+      <c r="E32" s="15" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D17" s="1"/>
-      <c r="E17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D18" s="1"/>
-      <c r="E18" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D19" s="1"/>
-      <c r="E19" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D20" s="1"/>
-      <c r="E20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D21" s="1"/>
-      <c r="E21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D22" s="1"/>
-      <c r="E22" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D23" s="1"/>
-      <c r="E23" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D24" s="1"/>
-      <c r="E24" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D25" s="1"/>
-      <c r="E25" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="D26" s="1"/>
-      <c r="E26" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E27" s="1" t="s">
+      <c r="F32" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.2">
-      <c r="E28" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>18</v>
+      <c r="G32" s="15">
+        <v>1</v>
+      </c>
+      <c r="H32" s="7"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="13"/>
+      <c r="M32" s="2"/>
+      <c r="N32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="P32" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="H17:H32"/>
+    <mergeCell ref="I31:K32"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>